<commit_message>
Add scraping more pages for each keyword
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,116 +455,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.aliexpress.com/item/1005003206531485.html?algo_pvid=e018906c-2ff1-4143-9967-934462a753b2&amp;algo_exp_id=e018906c-2ff1-4143-9967-934462a753b2-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000024658756093%22%7D&amp;pdp_pi=-1%3B6.38%3B-1%3B-1%40salePrice%3BEUR%3Bsearch-mainSearch</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>HARKO</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>aqua aquabeads</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://www.aliexpress.com/item/1005003044145843.html?algo_pvid=e018906c-2ff1-4143-9967-934462a753b2&amp;algo_exp_id=e018906c-2ff1-4143-9967-934462a753b2-1&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000023421416695%22%7D&amp;pdp_pi=-1%3B11.83%3B-1%3B35%40salePrice%3BEUR%3Bsearch-mainSearch</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://www.aliexpress.com/item/1005002905214870.html?algo_pvid=e018906c-2ff1-4143-9967-934462a753b2&amp;algo_exp_id=e018906c-2ff1-4143-9967-934462a753b2-2&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000022705782003%22%7D&amp;pdp_pi=-1%3B7.05%3B-1%3B192%40salePrice%3BEUR%3Bsearch-mainSearch</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>OLOEY</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://www.aliexpress.com/item/1005002709295207.html?algo_pvid=e018906c-2ff1-4143-9967-934462a753b2&amp;algo_exp_id=e018906c-2ff1-4143-9967-934462a753b2-3&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000021809007417%22%7D&amp;pdp_pi=-1%3B21.05%3B-1%3B-1%40salePrice%3BEUR%3Bsearch-mainSearch</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>HANDSHAKE FLEET</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://www.aliexpress.com/item/1005003155748447.html?algo_pvid=e018906c-2ff1-4143-9967-934462a753b2&amp;algo_exp_id=e018906c-2ff1-4143-9967-934462a753b2-4&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000024403877393%22%7D&amp;pdp_pi=-1%3B11.07%3B-1%3B-1%40salePrice%3BEUR%3Bsearch-mainSearch</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>QWZ</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>